<commit_message>
added excel data source
</commit_message>
<xml_diff>
--- a/EvomatixChecker/Data/loginData.xlsx
+++ b/EvomatixChecker/Data/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdhhewapathirana/Storage/Projects/evomatix/checkerCSharp/EvomatixChecker/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74BD3EC-8072-D64F-820E-7495D174FD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338ED2C3-A75D-CD4D-9F65-68FFDC65FB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{E7B20D56-BD6A-4C4C-9957-22BE7F2A9F91}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>passworrd</t>
-  </si>
-  <si>
     <t>admin1</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>admin4</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,12 +425,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>123</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>234</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>345</v>
@@ -454,7 +454,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>456</v>

</xml_diff>